<commit_message>
Correct bug in updating to 2015
</commit_message>
<xml_diff>
--- a/input/mappings/BP_2016_iso_mapping.xlsx
+++ b/input/mappings/BP_2016_iso_mapping.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="120" windowWidth="8440" windowHeight="20160" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="120" windowWidth="15260" windowHeight="20200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BP_2016_iso_mapping.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BP_2016_iso_mapping.csv!$A$1:$C$228</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BP_2016_iso_mapping.csv!$A$1:$C$227</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="294">
   <si>
     <t>iso</t>
   </si>
@@ -343,12 +343,6 @@
   </si>
   <si>
     <t>gin</t>
-  </si>
-  <si>
-    <t>global</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
   <si>
     <t>glp</t>
@@ -1414,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C228"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107:XFD107"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:XFD78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1434,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2272,23 +2266,26 @@
         <v>107</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>3</v>
+      </c>
+      <c r="C78" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B79" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
@@ -2299,7 +2296,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -2310,13 +2307,13 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" t="s">
         <v>112</v>
       </c>
-      <c r="B82" t="s">
-        <v>7</v>
-      </c>
       <c r="C82" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2324,34 +2321,34 @@
         <v>113</v>
       </c>
       <c r="B83" t="s">
-        <v>114</v>
+        <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>115</v>
-      </c>
-      <c r="B84" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="C84" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B86" t="s">
         <v>3</v>
@@ -2362,10 +2359,7 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>118</v>
-      </c>
-      <c r="B87" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="C87" t="s">
         <v>3</v>
@@ -2373,7 +2367,10 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3</v>
       </c>
       <c r="C88" t="s">
         <v>3</v>
@@ -2381,13 +2378,13 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
+        <v>119</v>
+      </c>
+      <c r="B89" t="s">
         <v>120</v>
       </c>
-      <c r="B89" t="s">
-        <v>3</v>
-      </c>
       <c r="C89" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2395,43 +2392,43 @@
         <v>121</v>
       </c>
       <c r="B90" t="s">
-        <v>122</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B91" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B92" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
+        <v>124</v>
+      </c>
+      <c r="B93" t="s">
         <v>125</v>
       </c>
-      <c r="B93" t="s">
-        <v>3</v>
-      </c>
       <c r="C93" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2442,7 +2439,7 @@
         <v>127</v>
       </c>
       <c r="C94" t="s">
-        <v>9</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2464,7 +2461,7 @@
         <v>131</v>
       </c>
       <c r="C96" t="s">
-        <v>131</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2475,7 +2472,7 @@
         <v>133</v>
       </c>
       <c r="C97" t="s">
-        <v>9</v>
+        <v>133</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2483,32 +2480,32 @@
         <v>134</v>
       </c>
       <c r="B98" t="s">
-        <v>135</v>
+        <v>34</v>
       </c>
       <c r="C98" t="s">
-        <v>135</v>
+        <v>34</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B99" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
+        <v>136</v>
+      </c>
+      <c r="B100" t="s">
         <v>137</v>
       </c>
-      <c r="B100" t="s">
-        <v>9</v>
-      </c>
       <c r="C100" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2519,7 +2516,7 @@
         <v>139</v>
       </c>
       <c r="C101" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2527,32 +2524,32 @@
         <v>140</v>
       </c>
       <c r="B102" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B103" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C103" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
+        <v>142</v>
+      </c>
+      <c r="B104" t="s">
         <v>143</v>
       </c>
-      <c r="B104" t="s">
-        <v>34</v>
-      </c>
       <c r="C104" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2560,37 +2557,37 @@
         <v>144</v>
       </c>
       <c r="B105" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="C105" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B106" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C106" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B107" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C107" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B108" t="s">
         <v>16</v>
@@ -2601,18 +2598,18 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B109" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B110" t="s">
         <v>5</v>
@@ -2623,24 +2620,24 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
+        <v>150</v>
+      </c>
+      <c r="B112" t="s">
         <v>151</v>
       </c>
-      <c r="B112" t="s">
-        <v>3</v>
-      </c>
       <c r="C112" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2651,7 +2648,7 @@
         <v>153</v>
       </c>
       <c r="C113" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2659,37 +2656,37 @@
         <v>154</v>
       </c>
       <c r="B114" t="s">
-        <v>155</v>
+        <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>155</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C115" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B116" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C116" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B117" t="s">
         <v>7</v>
@@ -2700,54 +2697,54 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B118" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C118" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>160</v>
-      </c>
-      <c r="B119" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="C119" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>161</v>
+        <v>160</v>
+      </c>
+      <c r="B120" t="s">
+        <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C121" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
+        <v>162</v>
+      </c>
+      <c r="B122" t="s">
         <v>163</v>
       </c>
-      <c r="B122" t="s">
-        <v>7</v>
-      </c>
       <c r="C122" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2755,7 +2752,7 @@
         <v>164</v>
       </c>
       <c r="B123" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
       <c r="C123" t="s">
         <v>9</v>
@@ -2763,7 +2760,7 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B124" t="s">
         <v>9</v>
@@ -2774,68 +2771,68 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B125" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C126" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B127" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C127" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B128" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B129" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
+        <v>171</v>
+      </c>
+      <c r="B130" t="s">
         <v>172</v>
       </c>
-      <c r="B130" t="s">
-        <v>5</v>
-      </c>
       <c r="C130" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2843,92 +2840,92 @@
         <v>173</v>
       </c>
       <c r="B131" t="s">
-        <v>174</v>
+        <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>174</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B132" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C132" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B133" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C133" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B134" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C134" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B135" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C136" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B137" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C137" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B138" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C138" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B139" t="s">
         <v>7</v>
@@ -2939,18 +2936,18 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B140" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C140" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B141" t="s">
         <v>3</v>
@@ -2961,18 +2958,18 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B142" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C142" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B143" t="s">
         <v>7</v>
@@ -2983,13 +2980,13 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
+        <v>186</v>
+      </c>
+      <c r="B144" t="s">
         <v>187</v>
       </c>
-      <c r="B144" t="s">
-        <v>7</v>
-      </c>
       <c r="C144" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2997,37 +2994,37 @@
         <v>188</v>
       </c>
       <c r="B145" t="s">
-        <v>189</v>
+        <v>7</v>
       </c>
       <c r="C145" t="s">
-        <v>189</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B146" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C146" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B147" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C147" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B148" t="s">
         <v>7</v>
@@ -3038,35 +3035,35 @@
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C149" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B150" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C150" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
+        <v>194</v>
+      </c>
+      <c r="B151" t="s">
         <v>195</v>
       </c>
-      <c r="B151" t="s">
-        <v>5</v>
-      </c>
       <c r="C151" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -3077,7 +3074,7 @@
         <v>197</v>
       </c>
       <c r="C152" t="s">
-        <v>9</v>
+        <v>197</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -3085,18 +3082,18 @@
         <v>198</v>
       </c>
       <c r="B153" t="s">
-        <v>199</v>
+        <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>199</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
+        <v>199</v>
+      </c>
+      <c r="B154" t="s">
         <v>200</v>
-      </c>
-      <c r="B154" t="s">
-        <v>5</v>
       </c>
       <c r="C154" t="s">
         <v>5</v>
@@ -3107,18 +3104,18 @@
         <v>201</v>
       </c>
       <c r="B155" t="s">
-        <v>202</v>
+        <v>34</v>
       </c>
       <c r="C155" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
+        <v>202</v>
+      </c>
+      <c r="B156" t="s">
         <v>203</v>
-      </c>
-      <c r="B156" t="s">
-        <v>34</v>
       </c>
       <c r="C156" t="s">
         <v>34</v>
@@ -3129,21 +3126,21 @@
         <v>204</v>
       </c>
       <c r="B157" t="s">
-        <v>205</v>
+        <v>3</v>
       </c>
       <c r="C157" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
+        <v>205</v>
+      </c>
+      <c r="B158" t="s">
         <v>206</v>
       </c>
-      <c r="B158" t="s">
-        <v>3</v>
-      </c>
       <c r="C158" t="s">
-        <v>3</v>
+        <v>206</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -3154,7 +3151,7 @@
         <v>208</v>
       </c>
       <c r="C159" t="s">
-        <v>208</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -3162,7 +3159,7 @@
         <v>209</v>
       </c>
       <c r="B160" t="s">
-        <v>210</v>
+        <v>5</v>
       </c>
       <c r="C160" t="s">
         <v>5</v>
@@ -3170,7 +3167,7 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B161" t="s">
         <v>5</v>
@@ -3181,13 +3178,13 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
+        <v>211</v>
+      </c>
+      <c r="B162" t="s">
         <v>212</v>
       </c>
-      <c r="B162" t="s">
-        <v>5</v>
-      </c>
-      <c r="C162" t="s">
-        <v>5</v>
+      <c r="C162" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3195,32 +3192,32 @@
         <v>213</v>
       </c>
       <c r="B163" t="s">
-        <v>214</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C163" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B164" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C164" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
+        <v>215</v>
+      </c>
+      <c r="B165" t="s">
         <v>216</v>
       </c>
-      <c r="B165" t="s">
-        <v>5</v>
-      </c>
       <c r="C165" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3228,32 +3225,32 @@
         <v>217</v>
       </c>
       <c r="B166" t="s">
-        <v>218</v>
+        <v>3</v>
       </c>
       <c r="C166" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B167" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
+        <v>219</v>
+      </c>
+      <c r="B168" t="s">
         <v>220</v>
       </c>
-      <c r="B168" t="s">
-        <v>5</v>
-      </c>
       <c r="C168" t="s">
-        <v>5</v>
+        <v>220</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3261,21 +3258,21 @@
         <v>221</v>
       </c>
       <c r="B169" t="s">
-        <v>222</v>
+        <v>7</v>
       </c>
       <c r="C169" t="s">
-        <v>222</v>
+        <v>7</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
+        <v>222</v>
+      </c>
+      <c r="B170" t="s">
         <v>223</v>
       </c>
-      <c r="B170" t="s">
-        <v>7</v>
-      </c>
       <c r="C170" t="s">
-        <v>7</v>
+        <v>223</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3283,32 +3280,32 @@
         <v>224</v>
       </c>
       <c r="B171" t="s">
-        <v>225</v>
+        <v>16</v>
       </c>
       <c r="C171" t="s">
-        <v>225</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B172" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C172" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
+        <v>226</v>
+      </c>
+      <c r="B173" t="s">
         <v>227</v>
       </c>
-      <c r="B173" t="s">
-        <v>7</v>
-      </c>
       <c r="C173" t="s">
-        <v>7</v>
+        <v>227</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3316,26 +3313,26 @@
         <v>228</v>
       </c>
       <c r="B174" t="s">
-        <v>229</v>
+        <v>9</v>
       </c>
       <c r="C174" t="s">
-        <v>229</v>
+        <v>9</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B175" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C175" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B176" t="s">
         <v>7</v>
@@ -3346,13 +3343,13 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
+        <v>231</v>
+      </c>
+      <c r="B177" t="s">
         <v>232</v>
       </c>
-      <c r="B177" t="s">
-        <v>7</v>
-      </c>
       <c r="C177" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3360,7 +3357,7 @@
         <v>233</v>
       </c>
       <c r="B178" t="s">
-        <v>234</v>
+        <v>5</v>
       </c>
       <c r="C178" t="s">
         <v>5</v>
@@ -3368,62 +3365,62 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B179" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C179" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B180" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C180" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B181" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C181" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B182" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C182" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B183" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C183" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>292</v>
       </c>
       <c r="B184" t="s">
         <v>9</v>
@@ -3434,35 +3431,35 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>294</v>
+        <v>239</v>
       </c>
       <c r="B185" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C185" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B186" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C186" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
+        <v>241</v>
+      </c>
+      <c r="B187" t="s">
         <v>242</v>
       </c>
-      <c r="B187" t="s">
-        <v>3</v>
-      </c>
-      <c r="C187" t="s">
-        <v>3</v>
+      <c r="C187" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3470,15 +3467,15 @@
         <v>243</v>
       </c>
       <c r="B188" t="s">
-        <v>244</v>
-      </c>
-      <c r="C188" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C188" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B189" t="s">
         <v>9</v>
@@ -3489,12 +3486,12 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
+        <v>244</v>
+      </c>
+      <c r="B190" t="s">
         <v>245</v>
       </c>
-      <c r="B190" t="s">
-        <v>9</v>
-      </c>
-      <c r="C190" t="s">
+      <c r="C190" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3503,70 +3500,70 @@
         <v>246</v>
       </c>
       <c r="B191" t="s">
-        <v>247</v>
-      </c>
-      <c r="C191" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C191" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B192" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C192" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B193" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C193" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B194" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C194" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B195" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C195" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B196" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C196" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B197" t="s">
         <v>7</v>
@@ -3577,13 +3574,13 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
+        <v>253</v>
+      </c>
+      <c r="B198" t="s">
         <v>254</v>
       </c>
-      <c r="B198" t="s">
-        <v>7</v>
-      </c>
       <c r="C198" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3591,48 +3588,48 @@
         <v>255</v>
       </c>
       <c r="B199" t="s">
-        <v>256</v>
+        <v>16</v>
       </c>
       <c r="C199" t="s">
-        <v>256</v>
+        <v>16</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B200" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C200" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B201" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C201" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B202" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C202" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B203" t="s">
         <v>5</v>
@@ -3643,13 +3640,13 @@
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
+        <v>260</v>
+      </c>
+      <c r="B204" t="s">
         <v>261</v>
       </c>
-      <c r="B204" t="s">
-        <v>5</v>
-      </c>
       <c r="C204" t="s">
-        <v>5</v>
+        <v>261</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3657,21 +3654,21 @@
         <v>262</v>
       </c>
       <c r="B205" t="s">
-        <v>263</v>
+        <v>7</v>
       </c>
       <c r="C205" t="s">
-        <v>263</v>
+        <v>7</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
+        <v>263</v>
+      </c>
+      <c r="B206" t="s">
         <v>264</v>
       </c>
-      <c r="B206" t="s">
-        <v>7</v>
-      </c>
-      <c r="C206" t="s">
-        <v>7</v>
+      <c r="C206" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3681,8 +3678,8 @@
       <c r="B207" t="s">
         <v>266</v>
       </c>
-      <c r="C207" s="1" t="s">
-        <v>9</v>
+      <c r="C207" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3690,15 +3687,15 @@
         <v>267</v>
       </c>
       <c r="B208" t="s">
-        <v>268</v>
+        <v>7</v>
       </c>
       <c r="C208" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B209" t="s">
         <v>7</v>
@@ -3709,35 +3706,35 @@
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B210" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C210" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B211" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C211" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
+        <v>271</v>
+      </c>
+      <c r="B212" t="s">
         <v>272</v>
       </c>
-      <c r="B212" t="s">
-        <v>3</v>
-      </c>
       <c r="C212" t="s">
-        <v>3</v>
+        <v>272</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3756,32 +3753,32 @@
         <v>275</v>
       </c>
       <c r="B214" t="s">
-        <v>276</v>
+        <v>16</v>
       </c>
       <c r="C214" t="s">
-        <v>276</v>
+        <v>16</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B215" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C215" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
+        <v>277</v>
+      </c>
+      <c r="B216" t="s">
         <v>278</v>
       </c>
-      <c r="B216" t="s">
-        <v>3</v>
-      </c>
       <c r="C216" t="s">
-        <v>3</v>
+        <v>278</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3789,15 +3786,15 @@
         <v>279</v>
       </c>
       <c r="B217" t="s">
-        <v>280</v>
+        <v>3</v>
       </c>
       <c r="C217" t="s">
-        <v>280</v>
+        <v>3</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B218" t="s">
         <v>3</v>
@@ -3808,13 +3805,13 @@
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
+        <v>281</v>
+      </c>
+      <c r="B219" t="s">
         <v>282</v>
       </c>
-      <c r="B219" t="s">
-        <v>3</v>
-      </c>
       <c r="C219" t="s">
-        <v>3</v>
+        <v>282</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3822,15 +3819,15 @@
         <v>283</v>
       </c>
       <c r="B220" t="s">
-        <v>284</v>
+        <v>5</v>
       </c>
       <c r="C220" t="s">
-        <v>284</v>
+        <v>5</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B221" t="s">
         <v>5</v>
@@ -3841,7 +3838,7 @@
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B222" t="s">
         <v>5</v>
@@ -3852,35 +3849,35 @@
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B223" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C223" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>288</v>
-      </c>
-      <c r="B224" t="s">
-        <v>34</v>
-      </c>
-      <c r="C224" t="s">
-        <v>34</v>
+        <v>287</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
+        <v>288</v>
+      </c>
+      <c r="B225" t="s">
         <v>289</v>
       </c>
-      <c r="B225" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>9</v>
+      <c r="C225" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3888,7 +3885,7 @@
         <v>290</v>
       </c>
       <c r="B226" t="s">
-        <v>291</v>
+        <v>7</v>
       </c>
       <c r="C226" t="s">
         <v>7</v>
@@ -3896,7 +3893,7 @@
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B227" t="s">
         <v>7</v>
@@ -3905,19 +3902,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
-      <c r="A228" t="s">
-        <v>293</v>
-      </c>
-      <c r="B228" t="s">
-        <v>7</v>
-      </c>
-      <c r="C228" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C228">
+  <autoFilter ref="A1:C227">
     <sortState ref="A2:C238">
       <sortCondition ref="A2"/>
     </sortState>

</xml_diff>

<commit_message>
Add ssd (South Sudan) to BP mapping 2016 Fix data input error in BP extension
</commit_message>
<xml_diff>
--- a/input/mappings/BP_2016_iso_mapping.xlsx
+++ b/input/mappings/BP_2016_iso_mapping.xlsx
@@ -10,7 +10,7 @@
     <sheet name="BP_2016_iso_mapping.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BP_2016_iso_mapping.csv!$A$1:$C$227</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BP_2016_iso_mapping.csv!$A$1:$C$228</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="295">
   <si>
     <t>iso</t>
   </si>
@@ -904,6 +904,9 @@
   </si>
   <si>
     <t>BPName_2016_Oil</t>
+  </si>
+  <si>
+    <t>ssd</t>
   </si>
 </sst>
 </file>
@@ -1408,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C227"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD78"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3431,7 +3434,7 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>239</v>
+        <v>294</v>
       </c>
       <c r="B185" t="s">
         <v>7</v>
@@ -3442,34 +3445,34 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B186" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C186" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B187" t="s">
-        <v>242</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C187" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B188" t="s">
-        <v>9</v>
-      </c>
-      <c r="C188" t="s">
+        <v>242</v>
+      </c>
+      <c r="C188" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3486,84 +3489,84 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B190" t="s">
-        <v>245</v>
-      </c>
-      <c r="C190" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C190" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B191" t="s">
-        <v>7</v>
-      </c>
-      <c r="C191" t="s">
-        <v>7</v>
+        <v>245</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B192" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C192" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B193" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C193" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B194" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C194" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B195" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C195" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B196" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C196" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B197" t="s">
         <v>7</v>
@@ -3574,62 +3577,62 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B198" t="s">
-        <v>254</v>
+        <v>7</v>
       </c>
       <c r="C198" t="s">
-        <v>254</v>
+        <v>7</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B199" t="s">
-        <v>16</v>
+        <v>254</v>
       </c>
       <c r="C199" t="s">
-        <v>16</v>
+        <v>254</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B200" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C200" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B201" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C201" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B202" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C202" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B203" t="s">
         <v>5</v>
@@ -3640,62 +3643,62 @@
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B204" t="s">
-        <v>261</v>
+        <v>5</v>
       </c>
       <c r="C204" t="s">
-        <v>261</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B205" t="s">
-        <v>7</v>
+        <v>261</v>
       </c>
       <c r="C205" t="s">
-        <v>7</v>
+        <v>261</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B206" t="s">
-        <v>264</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C206" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B207" t="s">
-        <v>266</v>
-      </c>
-      <c r="C207" t="s">
-        <v>5</v>
+        <v>264</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B208" t="s">
-        <v>7</v>
+        <v>266</v>
       </c>
       <c r="C208" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B209" t="s">
         <v>7</v>
@@ -3706,95 +3709,95 @@
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B210" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C210" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B211" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C211" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B212" t="s">
-        <v>272</v>
+        <v>3</v>
       </c>
       <c r="C212" t="s">
-        <v>272</v>
+        <v>3</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B213" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C213" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B214" t="s">
-        <v>16</v>
+        <v>274</v>
       </c>
       <c r="C214" t="s">
-        <v>16</v>
+        <v>274</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B215" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C215" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B216" t="s">
-        <v>278</v>
+        <v>3</v>
       </c>
       <c r="C216" t="s">
-        <v>278</v>
+        <v>3</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B217" t="s">
-        <v>3</v>
+        <v>278</v>
       </c>
       <c r="C217" t="s">
-        <v>3</v>
+        <v>278</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B218" t="s">
         <v>3</v>
@@ -3805,29 +3808,29 @@
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B219" t="s">
-        <v>282</v>
+        <v>3</v>
       </c>
       <c r="C219" t="s">
-        <v>282</v>
+        <v>3</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B220" t="s">
-        <v>5</v>
+        <v>282</v>
       </c>
       <c r="C220" t="s">
-        <v>5</v>
+        <v>282</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B221" t="s">
         <v>5</v>
@@ -3838,7 +3841,7 @@
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B222" t="s">
         <v>5</v>
@@ -3849,43 +3852,43 @@
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B223" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C223" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>287</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C224" s="1" t="s">
-        <v>9</v>
+        <v>286</v>
+      </c>
+      <c r="B224" t="s">
+        <v>34</v>
+      </c>
+      <c r="C224" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>288</v>
-      </c>
-      <c r="B225" t="s">
-        <v>289</v>
-      </c>
-      <c r="C225" t="s">
-        <v>7</v>
+        <v>287</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B226" t="s">
-        <v>7</v>
+        <v>289</v>
       </c>
       <c r="C226" t="s">
         <v>7</v>
@@ -3893,17 +3896,28 @@
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
+        <v>290</v>
+      </c>
+      <c r="B227" t="s">
+        <v>7</v>
+      </c>
+      <c r="C227" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" t="s">
         <v>291</v>
       </c>
-      <c r="B227" t="s">
-        <v>7</v>
-      </c>
-      <c r="C227" t="s">
+      <c r="B228" t="s">
+        <v>7</v>
+      </c>
+      <c r="C228" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C227">
+  <autoFilter ref="A1:C228">
     <sortState ref="A2:C238">
       <sortCondition ref="A2"/>
     </sortState>

</xml_diff>

<commit_message>
Change mistake in mapping file (ssd)
</commit_message>
<xml_diff>
--- a/input/mappings/BP_2016_iso_mapping.xlsx
+++ b/input/mappings/BP_2016_iso_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="120" windowWidth="15260" windowHeight="20200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14660" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BP_2016_iso_mapping.csv" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="295">
   <si>
     <t>iso</t>
   </si>
@@ -1414,7 +1414,7 @@
   <dimension ref="A1:C228"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="B185" sqref="B185"/>
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3435,9 +3435,6 @@
     <row r="185" spans="1:3">
       <c r="A185" t="s">
         <v>294</v>
-      </c>
-      <c r="B185" t="s">
-        <v>7</v>
       </c>
       <c r="C185" t="s">
         <v>7</v>

</xml_diff>